<commit_message>
Updated with cement data, imported, and removed unused code.
</commit_message>
<xml_diff>
--- a/ree_data_r.xlsx
+++ b/ree_data_r.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailmissouri-my.sharepoint.com/personal/ckwr82_umsystem_edu/Documents/Documents/Research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailmissouri-my.sharepoint.com/personal/ckwr82_umsystem_edu/Documents/Documents/Research/isotope and REY files/REY/fu-rey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="8_{31468CF1-D59E-4952-A76B-1B79FB8CF6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AA4BA8C-48E0-41E2-8F67-9B0B6D17A84F}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="8_{31468CF1-D59E-4952-A76B-1B79FB8CF6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF7D89CC-CCE6-41A9-9724-3DD7104F77ED}"/>
   <bookViews>
-    <workbookView xWindow="2475" yWindow="900" windowWidth="14820" windowHeight="13380" xr2:uid="{BF2FDE4A-2A08-4690-AA86-00AFD658EF24}"/>
+    <workbookView xWindow="8235" yWindow="270" windowWidth="14820" windowHeight="14340" activeTab="1" xr2:uid="{BF2FDE4A-2A08-4690-AA86-00AFD658EF24}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="cements" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="66">
   <si>
     <t>Sample</t>
   </si>
@@ -214,6 +215,30 @@
   <si>
     <t>U_ppm</t>
   </si>
+  <si>
+    <t>Cement</t>
+  </si>
+  <si>
+    <t>Micrite (SSF)</t>
+  </si>
+  <si>
+    <t>Micrite</t>
+  </si>
+  <si>
+    <t>Laminar Calcrete</t>
+  </si>
+  <si>
+    <t>Laminar Microbial</t>
+  </si>
+  <si>
+    <t>Manganese</t>
+  </si>
+  <si>
+    <t>Microbial (SSF)</t>
+  </si>
+  <si>
+    <t>Microbial</t>
+  </si>
 </sst>
 </file>
 
@@ -268,7 +293,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="original data"/>
@@ -3058,8 +3083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C554F00-4C65-4A12-A3F1-5137239F542B}">
   <dimension ref="A1:AF27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6497,4 +6522,238 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F2BC39-F234-4290-807E-B62380110B4E}">
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added data from rerunning samples with sequential leach
</commit_message>
<xml_diff>
--- a/ree_data_r.xlsx
+++ b/ree_data_r.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailmissouri-my.sharepoint.com/personal/ckwr82_umsystem_edu/Documents/Documents/Research/isotope and REY files/REY/fu-rey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="8_{31468CF1-D59E-4952-A76B-1B79FB8CF6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF7D89CC-CCE6-41A9-9724-3DD7104F77ED}"/>
+  <xr:revisionPtr revIDLastSave="122" documentId="8_{31468CF1-D59E-4952-A76B-1B79FB8CF6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D881A311-C858-4E5A-AAA3-9113A6F4305E}"/>
   <bookViews>
-    <workbookView xWindow="8235" yWindow="270" windowWidth="14820" windowHeight="14340" activeTab="1" xr2:uid="{BF2FDE4A-2A08-4690-AA86-00AFD658EF24}"/>
+    <workbookView xWindow="5685" yWindow="3435" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{BF2FDE4A-2A08-4690-AA86-00AFD658EF24}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="82">
   <si>
     <t>Sample</t>
   </si>
@@ -238,6 +238,54 @@
   </si>
   <si>
     <t>Microbial</t>
+  </si>
+  <si>
+    <t>FUWM 1 3 dil</t>
+  </si>
+  <si>
+    <t>FUWM 3.5 H 1 dil</t>
+  </si>
+  <si>
+    <t>FUWM 3.5 H 2 dil</t>
+  </si>
+  <si>
+    <t>FUWM 8.5 2 dil</t>
+  </si>
+  <si>
+    <t>FUWM 8.5 3 dil</t>
+  </si>
+  <si>
+    <t>FUWM 16 T 4 dil</t>
+  </si>
+  <si>
+    <t>FUWM 16 T 5 dil</t>
+  </si>
+  <si>
+    <t>FUWM 3.5 T 1</t>
+  </si>
+  <si>
+    <t>FUWM 3.5 T 2</t>
+  </si>
+  <si>
+    <t>FUWM 3.5 T 3</t>
+  </si>
+  <si>
+    <t>FUWM 3.5 T 5</t>
+  </si>
+  <si>
+    <t>FUWM 3 A 1</t>
+  </si>
+  <si>
+    <t>Micrite Above</t>
+  </si>
+  <si>
+    <t>FUWM 4 1.5m B</t>
+  </si>
+  <si>
+    <t>FUWM 4 3m B</t>
+  </si>
+  <si>
+    <t>Micrite Below</t>
   </si>
 </sst>
 </file>
@@ -2782,6 +2830,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6526,15 +6578,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F2BC39-F234-4290-807E-B62380110B4E}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -6571,47 +6623,47 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>61</v>
@@ -6619,7 +6671,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>62</v>
@@ -6627,15 +6679,15 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
         <v>59</v>
@@ -6643,113 +6695,225 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>80</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B41" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added old dataset to rerun data file, edited old data excel sheet to exclude an element that was not detected, updated gitignore to ignore png
</commit_message>
<xml_diff>
--- a/ree_data_r.xlsx
+++ b/ree_data_r.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailmissouri-my.sharepoint.com/personal/ckwr82_umsystem_edu/Documents/Documents/Research/isotope and REY files/REY/fu-rey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="122" documentId="8_{31468CF1-D59E-4952-A76B-1B79FB8CF6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D881A311-C858-4E5A-AAA3-9113A6F4305E}"/>
+  <xr:revisionPtr revIDLastSave="123" documentId="8_{31468CF1-D59E-4952-A76B-1B79FB8CF6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8257B2C8-5C0E-4BA1-8671-FAAC385FEC8A}"/>
   <bookViews>
-    <workbookView xWindow="5685" yWindow="3435" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{BF2FDE4A-2A08-4690-AA86-00AFD658EF24}"/>
+    <workbookView xWindow="-1425" yWindow="990" windowWidth="21600" windowHeight="11385" xr2:uid="{BF2FDE4A-2A08-4690-AA86-00AFD658EF24}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="81">
   <si>
     <t>Sample</t>
   </si>
@@ -163,9 +163,6 @@
   </si>
   <si>
     <t>Mo_ppm</t>
-  </si>
-  <si>
-    <t>In_ppm</t>
   </si>
   <si>
     <t>Ba_ppm</t>
@@ -3133,10 +3130,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C554F00-4C65-4A12-A3F1-5137239F542B}">
-  <dimension ref="A1:AF27"/>
+  <dimension ref="A1:AE27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3152,26 +3149,25 @@
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3265,11 +3261,8 @@
       <c r="AE1" t="s">
         <v>56</v>
       </c>
-      <c r="AF1" t="s">
-        <v>57</v>
-      </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3330,73 +3323,70 @@
         <v>217.01786264896649</v>
       </c>
       <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q3*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG3))/'[1]Formula (ppm) Duplicates Remove'!$AH3</f>
         <v>21.2317092124627</v>
       </c>
-      <c r="R2">
+      <c r="Q2">
         <f>'[1]Formula (ppm) Duplicates Remove'!R3*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG3))/'[1]Formula (ppm) Duplicates Remove'!$AH3</f>
         <v>6.1153832254056777</v>
       </c>
-      <c r="S2">
+      <c r="R2">
         <f>'[1]Formula (ppm) Duplicates Remove'!S3*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG3))/'[1]Formula (ppm) Duplicates Remove'!$AH3</f>
         <v>62.524629517479347</v>
       </c>
-      <c r="T2">
+      <c r="S2">
         <f>'[1]Formula (ppm) Duplicates Remove'!T3*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG3))/'[1]Formula (ppm) Duplicates Remove'!$AH3</f>
         <v>1.5523183622319427</v>
       </c>
-      <c r="U2">
+      <c r="T2">
         <f>'[1]Formula (ppm) Duplicates Remove'!U3*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG3))/'[1]Formula (ppm) Duplicates Remove'!$AH3</f>
         <v>6.6849839147730457</v>
       </c>
-      <c r="V2">
+      <c r="U2">
         <f>'[1]Formula (ppm) Duplicates Remove'!V3*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG3))/'[1]Formula (ppm) Duplicates Remove'!$AH3</f>
         <v>1.4459094422402372</v>
       </c>
-      <c r="W2">
+      <c r="V2">
         <f>'[1]Formula (ppm) Duplicates Remove'!W3*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG3))/'[1]Formula (ppm) Duplicates Remove'!$AH3</f>
         <v>0.29418936703589238</v>
       </c>
-      <c r="X2">
+      <c r="W2">
         <f>'[1]Formula (ppm) Duplicates Remove'!X3*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG3))/'[1]Formula (ppm) Duplicates Remove'!$AH3</f>
         <v>1.8277296845634166</v>
       </c>
-      <c r="Y2">
+      <c r="X2">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y3*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG3))/'[1]Formula (ppm) Duplicates Remove'!$AH3</f>
         <v>1.5460590139971364</v>
       </c>
-      <c r="Z2">
+      <c r="Y2">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z3*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG3))/'[1]Formula (ppm) Duplicates Remove'!$AH3</f>
         <v>0.40685763526240437</v>
       </c>
-      <c r="AA2">
+      <c r="Z2">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA3*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG3))/'[1]Formula (ppm) Duplicates Remove'!$AH3</f>
         <v>0.97645832462977045</v>
       </c>
-      <c r="AB2">
+      <c r="AA2">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB3*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG3))/'[1]Formula (ppm) Duplicates Remove'!$AH3</f>
         <v>0.13770566116573685</v>
       </c>
-      <c r="AC2">
+      <c r="AB2">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC3*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG3))/'[1]Formula (ppm) Duplicates Remove'!$AH3</f>
         <v>0.91386484228170828</v>
       </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
       <c r="AD2">
-        <v>0</v>
-      </c>
-      <c r="AE2">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE3*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG3))/'[1]Formula (ppm) Duplicates Remove'!$AH3</f>
         <v>3.2798984750384599</v>
       </c>
-      <c r="AF2">
+      <c r="AE2">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF3*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG3))/'[1]Formula (ppm) Duplicates Remove'!$AH3</f>
         <v>0.18152109880938042</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3457,73 +3447,70 @@
         <v>178.78639468039864</v>
       </c>
       <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q4*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG4))/'[1]Formula (ppm) Duplicates Remove'!$AH4</f>
         <v>42.047126312654505</v>
       </c>
-      <c r="R3">
+      <c r="Q3">
         <f>'[1]Formula (ppm) Duplicates Remove'!R4*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG4))/'[1]Formula (ppm) Duplicates Remove'!$AH4</f>
         <v>4.6895660726779127</v>
       </c>
-      <c r="S3">
+      <c r="R3">
         <f>'[1]Formula (ppm) Duplicates Remove'!S4*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG4))/'[1]Formula (ppm) Duplicates Remove'!$AH4</f>
         <v>23.903539608870133</v>
       </c>
-      <c r="T3">
+      <c r="S3">
         <f>'[1]Formula (ppm) Duplicates Remove'!T4*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG4))/'[1]Formula (ppm) Duplicates Remove'!$AH4</f>
         <v>1.0332942194036079</v>
       </c>
-      <c r="U3">
+      <c r="T3">
         <f>'[1]Formula (ppm) Duplicates Remove'!U4*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG4))/'[1]Formula (ppm) Duplicates Remove'!$AH4</f>
         <v>4.276248384916471</v>
       </c>
-      <c r="V3">
+      <c r="U3">
         <f>'[1]Formula (ppm) Duplicates Remove'!V4*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG4))/'[1]Formula (ppm) Duplicates Remove'!$AH4</f>
         <v>0.90082060153135046</v>
       </c>
-      <c r="W3">
+      <c r="V3">
         <f>'[1]Formula (ppm) Duplicates Remove'!W4*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG4))/'[1]Formula (ppm) Duplicates Remove'!$AH4</f>
         <v>0.19606095445094096</v>
       </c>
-      <c r="X3">
+      <c r="W3">
         <f>'[1]Formula (ppm) Duplicates Remove'!X4*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG4))/'[1]Formula (ppm) Duplicates Remove'!$AH4</f>
         <v>1.0491910535482789</v>
       </c>
-      <c r="Y3">
+      <c r="X3">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y4*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG4))/'[1]Formula (ppm) Duplicates Remove'!$AH4</f>
         <v>0.81073854137821544</v>
       </c>
-      <c r="Z3">
+      <c r="Y3">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z4*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG4))/'[1]Formula (ppm) Duplicates Remove'!$AH4</f>
         <v>0.2119577885956119</v>
       </c>
-      <c r="AA3">
+      <c r="Z3">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA4*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG4))/'[1]Formula (ppm) Duplicates Remove'!$AH4</f>
         <v>0.47690502434012666</v>
       </c>
-      <c r="AB3">
+      <c r="AA3">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB4*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG4))/'[1]Formula (ppm) Duplicates Remove'!$AH4</f>
         <v>6.8886281293573853E-2</v>
       </c>
-      <c r="AC3">
+      <c r="AB3">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC4*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG4))/'[1]Formula (ppm) Duplicates Remove'!$AH4</f>
         <v>0.4027197983316626</v>
       </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
       <c r="AD3">
-        <v>0</v>
-      </c>
-      <c r="AE3">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE4*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG4))/'[1]Formula (ppm) Duplicates Remove'!$AH4</f>
         <v>3.2111604972235201</v>
       </c>
-      <c r="AF3">
+      <c r="AE3">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF4*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG4))/'[1]Formula (ppm) Duplicates Remove'!$AH4</f>
         <v>0.29674090403385661</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3584,73 +3571,70 @@
         <v>190.64358762566826</v>
       </c>
       <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q5*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG5))/'[1]Formula (ppm) Duplicates Remove'!$AH5</f>
         <v>20.102670390701263</v>
       </c>
-      <c r="R4">
+      <c r="Q4">
         <f>'[1]Formula (ppm) Duplicates Remove'!R5*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG5))/'[1]Formula (ppm) Duplicates Remove'!$AH5</f>
         <v>6.8423050193458295</v>
       </c>
-      <c r="S4">
+      <c r="R4">
         <f>'[1]Formula (ppm) Duplicates Remove'!S5*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG5))/'[1]Formula (ppm) Duplicates Remove'!$AH5</f>
         <v>21.087135580289171</v>
       </c>
-      <c r="T4">
+      <c r="S4">
         <f>'[1]Formula (ppm) Duplicates Remove'!T5*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG5))/'[1]Formula (ppm) Duplicates Remove'!$AH5</f>
         <v>1.240099796828974</v>
       </c>
-      <c r="U4">
+      <c r="T4">
         <f>'[1]Formula (ppm) Duplicates Remove'!U5*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG5))/'[1]Formula (ppm) Duplicates Remove'!$AH5</f>
         <v>5.1779605551806274</v>
       </c>
-      <c r="V4">
+      <c r="U4">
         <f>'[1]Formula (ppm) Duplicates Remove'!V5*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG5))/'[1]Formula (ppm) Duplicates Remove'!$AH5</f>
         <v>1.0062213263743867</v>
       </c>
-      <c r="W4">
+      <c r="V4">
         <f>'[1]Formula (ppm) Duplicates Remove'!W5*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG5))/'[1]Formula (ppm) Duplicates Remove'!$AH5</f>
         <v>0.21212233366811395</v>
       </c>
-      <c r="X4">
+      <c r="W4">
         <f>'[1]Formula (ppm) Duplicates Remove'!X5*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG5))/'[1]Formula (ppm) Duplicates Remove'!$AH5</f>
         <v>1.1748313864695541</v>
       </c>
-      <c r="Y4">
+      <c r="X4">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y5*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG5))/'[1]Formula (ppm) Duplicates Remove'!$AH5</f>
         <v>0.8974406424420206</v>
       </c>
-      <c r="Z4">
+      <c r="Y4">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z5*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG5))/'[1]Formula (ppm) Duplicates Remove'!$AH5</f>
         <v>0.23931750465120546</v>
       </c>
-      <c r="AA4">
+      <c r="Z4">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA5*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG5))/'[1]Formula (ppm) Duplicates Remove'!$AH5</f>
         <v>0.54390341966183076</v>
       </c>
-      <c r="AB4">
+      <c r="AA4">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB5*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG5))/'[1]Formula (ppm) Duplicates Remove'!$AH5</f>
         <v>7.6146478752656288E-2</v>
       </c>
-      <c r="AC4">
+      <c r="AB4">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC5*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG5))/'[1]Formula (ppm) Duplicates Remove'!$AH5</f>
         <v>0.46231790671255607</v>
       </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
       <c r="AD4">
-        <v>0</v>
-      </c>
-      <c r="AE4">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE5*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG5))/'[1]Formula (ppm) Duplicates Remove'!$AH5</f>
         <v>18.541667576271806</v>
       </c>
-      <c r="AF4">
+      <c r="AE4">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF5*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG5))/'[1]Formula (ppm) Duplicates Remove'!$AH5</f>
         <v>0.26651267563429704</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3711,73 +3695,70 @@
         <v>146.62273716465054</v>
       </c>
       <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q6*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG6))/'[1]Formula (ppm) Duplicates Remove'!$AH6</f>
         <v>2322.6477925278691</v>
       </c>
-      <c r="R5">
+      <c r="Q5">
         <f>'[1]Formula (ppm) Duplicates Remove'!R6*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG6))/'[1]Formula (ppm) Duplicates Remove'!$AH6</f>
         <v>17.635932750208941</v>
       </c>
-      <c r="S5">
+      <c r="R5">
         <f>'[1]Formula (ppm) Duplicates Remove'!S6*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG6))/'[1]Formula (ppm) Duplicates Remove'!$AH6</f>
         <v>181.50572683149591</v>
       </c>
-      <c r="T5">
+      <c r="S5">
         <f>'[1]Formula (ppm) Duplicates Remove'!T6*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG6))/'[1]Formula (ppm) Duplicates Remove'!$AH6</f>
         <v>3.93840205915996</v>
       </c>
-      <c r="U5">
+      <c r="T5">
         <f>'[1]Formula (ppm) Duplicates Remove'!U6*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG6))/'[1]Formula (ppm) Duplicates Remove'!$AH6</f>
         <v>15.794978006168833</v>
       </c>
-      <c r="V5">
+      <c r="U5">
         <f>'[1]Formula (ppm) Duplicates Remove'!V6*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG6))/'[1]Formula (ppm) Duplicates Remove'!$AH6</f>
         <v>3.3964580783301752</v>
       </c>
-      <c r="W5">
+      <c r="V5">
         <f>'[1]Formula (ppm) Duplicates Remove'!W6*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG6))/'[1]Formula (ppm) Duplicates Remove'!$AH6</f>
         <v>1.2535040167284326</v>
       </c>
-      <c r="X5">
+      <c r="W5">
         <f>'[1]Formula (ppm) Duplicates Remove'!X6*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG6))/'[1]Formula (ppm) Duplicates Remove'!$AH6</f>
         <v>4.3769216161672677</v>
       </c>
-      <c r="Y5">
+      <c r="X5">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y6*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG6))/'[1]Formula (ppm) Duplicates Remove'!$AH6</f>
         <v>3.578485064257737</v>
       </c>
-      <c r="Z5">
+      <c r="Y5">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z6*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG6))/'[1]Formula (ppm) Duplicates Remove'!$AH6</f>
         <v>0.88945004487331036</v>
       </c>
-      <c r="AA5">
+      <c r="Z5">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA6*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG6))/'[1]Formula (ppm) Duplicates Remove'!$AH6</f>
         <v>2.2712003471416153</v>
       </c>
-      <c r="AB5">
+      <c r="AA5">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB6*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG6))/'[1]Formula (ppm) Duplicates Remove'!$AH6</f>
         <v>0.33095815623192948</v>
       </c>
-      <c r="AC5">
+      <c r="AB5">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC6*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG6))/'[1]Formula (ppm) Duplicates Remove'!$AH6</f>
         <v>2.0933103381669538</v>
       </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
       <c r="AD5">
-        <v>0</v>
-      </c>
-      <c r="AE5">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE6*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG6))/'[1]Formula (ppm) Duplicates Remove'!$AH6</f>
         <v>8.3691043757149153</v>
       </c>
-      <c r="AF5">
+      <c r="AE5">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF6*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG6))/'[1]Formula (ppm) Duplicates Remove'!$AH6</f>
         <v>0.210985824597855</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3838,73 +3819,70 @@
         <v>183.58030840757945</v>
       </c>
       <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q7*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG7))/'[1]Formula (ppm) Duplicates Remove'!$AH7</f>
         <v>158.87930345572906</v>
       </c>
-      <c r="R6">
+      <c r="Q6">
         <f>'[1]Formula (ppm) Duplicates Remove'!R7*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG7))/'[1]Formula (ppm) Duplicates Remove'!$AH7</f>
         <v>31.620613073042158</v>
       </c>
-      <c r="S6">
+      <c r="R6">
         <f>'[1]Formula (ppm) Duplicates Remove'!S7*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG7))/'[1]Formula (ppm) Duplicates Remove'!$AH7</f>
         <v>252.62668655918279</v>
       </c>
-      <c r="T6">
+      <c r="S6">
         <f>'[1]Formula (ppm) Duplicates Remove'!T7*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG7))/'[1]Formula (ppm) Duplicates Remove'!$AH7</f>
         <v>7.4075292066604099</v>
       </c>
-      <c r="U6">
+      <c r="T6">
         <f>'[1]Formula (ppm) Duplicates Remove'!U7*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG7))/'[1]Formula (ppm) Duplicates Remove'!$AH7</f>
         <v>30.750117500103766</v>
       </c>
-      <c r="V6">
+      <c r="U6">
         <f>'[1]Formula (ppm) Duplicates Remove'!V7*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG7))/'[1]Formula (ppm) Duplicates Remove'!$AH7</f>
         <v>6.4649543824596076</v>
       </c>
-      <c r="W6">
+      <c r="V6">
         <f>'[1]Formula (ppm) Duplicates Remove'!W7*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG7))/'[1]Formula (ppm) Duplicates Remove'!$AH7</f>
         <v>1.3750503317752856</v>
       </c>
-      <c r="X6">
+      <c r="W6">
         <f>'[1]Formula (ppm) Duplicates Remove'!X7*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG7))/'[1]Formula (ppm) Duplicates Remove'!$AH7</f>
         <v>7.7901036941301465</v>
       </c>
-      <c r="Y6">
+      <c r="X6">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y7*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG7))/'[1]Formula (ppm) Duplicates Remove'!$AH7</f>
         <v>5.4447557492069771</v>
       </c>
-      <c r="Z6">
+      <c r="Y6">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z7*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG7))/'[1]Formula (ppm) Duplicates Remove'!$AH7</f>
         <v>1.3306938694599537</v>
       </c>
-      <c r="AA6">
+      <c r="Z6">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA7*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG7))/'[1]Formula (ppm) Duplicates Remove'!$AH7</f>
         <v>3.0605958997578941</v>
       </c>
-      <c r="AB6">
+      <c r="AA6">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB7*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG7))/'[1]Formula (ppm) Duplicates Remove'!$AH7</f>
         <v>0.41584183420623549</v>
       </c>
-      <c r="AC6">
+      <c r="AB6">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC7*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG7))/'[1]Formula (ppm) Duplicates Remove'!$AH7</f>
         <v>2.6392095077622413</v>
       </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
       <c r="AD6">
-        <v>0</v>
-      </c>
-      <c r="AE6">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE7*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG7))/'[1]Formula (ppm) Duplicates Remove'!$AH7</f>
         <v>12.97426522723455</v>
       </c>
-      <c r="AF6">
+      <c r="AE6">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF7*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG7))/'[1]Formula (ppm) Duplicates Remove'!$AH7</f>
         <v>0.34376258294382139</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -3965,73 +3943,70 @@
         <v>173.55067810886973</v>
       </c>
       <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q8*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG8))/'[1]Formula (ppm) Duplicates Remove'!$AH8</f>
         <v>14.774943824826998</v>
       </c>
-      <c r="R7">
+      <c r="Q7">
         <f>'[1]Formula (ppm) Duplicates Remove'!R8*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG8))/'[1]Formula (ppm) Duplicates Remove'!$AH8</f>
         <v>9.5229320787041534</v>
       </c>
-      <c r="S7">
+      <c r="R7">
         <f>'[1]Formula (ppm) Duplicates Remove'!S8*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG8))/'[1]Formula (ppm) Duplicates Remove'!$AH8</f>
         <v>52.764170051661665</v>
       </c>
-      <c r="T7">
+      <c r="S7">
         <f>'[1]Formula (ppm) Duplicates Remove'!T8*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG8))/'[1]Formula (ppm) Duplicates Remove'!$AH8</f>
         <v>1.942658619848413</v>
       </c>
-      <c r="U7">
+      <c r="T7">
         <f>'[1]Formula (ppm) Duplicates Remove'!U8*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG8))/'[1]Formula (ppm) Duplicates Remove'!$AH8</f>
         <v>7.7852776348196446</v>
       </c>
-      <c r="V7">
+      <c r="U7">
         <f>'[1]Formula (ppm) Duplicates Remove'!V8*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG8))/'[1]Formula (ppm) Duplicates Remove'!$AH8</f>
         <v>1.6156281486679012</v>
       </c>
-      <c r="W7">
+      <c r="V7">
         <f>'[1]Formula (ppm) Duplicates Remove'!W8*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG8))/'[1]Formula (ppm) Duplicates Remove'!$AH8</f>
         <v>0.32214941937184738</v>
       </c>
-      <c r="X7">
+      <c r="W7">
         <f>'[1]Formula (ppm) Duplicates Remove'!X8*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG8))/'[1]Formula (ppm) Duplicates Remove'!$AH8</f>
         <v>1.9670638788917347</v>
       </c>
-      <c r="Y7">
+      <c r="X7">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y8*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG8))/'[1]Formula (ppm) Duplicates Remove'!$AH8</f>
         <v>1.6302713040938941</v>
       </c>
-      <c r="Z7">
+      <c r="Y7">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z8*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG8))/'[1]Formula (ppm) Duplicates Remove'!$AH8</f>
         <v>0.43929466277979173</v>
       </c>
-      <c r="AA7">
+      <c r="Z7">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA8*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG8))/'[1]Formula (ppm) Duplicates Remove'!$AH8</f>
         <v>1.1079987605668082</v>
       </c>
-      <c r="AB7">
+      <c r="AA7">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB8*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG8))/'[1]Formula (ppm) Duplicates Remove'!$AH8</f>
         <v>0.16595576149458802</v>
       </c>
-      <c r="AC7">
+      <c r="AB7">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC8*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG8))/'[1]Formula (ppm) Duplicates Remove'!$AH8</f>
         <v>1.1470471750361231</v>
       </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
       <c r="AD7">
-        <v>0</v>
-      </c>
-      <c r="AE7">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE8*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG8))/'[1]Formula (ppm) Duplicates Remove'!$AH8</f>
         <v>22.291763610170101</v>
       </c>
-      <c r="AF7">
+      <c r="AE7">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF8*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG8))/'[1]Formula (ppm) Duplicates Remove'!$AH8</f>
         <v>0.79073039300362524</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -4092,73 +4067,70 @@
         <v>158.1332638554351</v>
       </c>
       <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q9*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG9))/'[1]Formula (ppm) Duplicates Remove'!$AH9</f>
         <v>31.893373357975523</v>
       </c>
-      <c r="R8">
+      <c r="Q8">
         <f>'[1]Formula (ppm) Duplicates Remove'!R9*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG9))/'[1]Formula (ppm) Duplicates Remove'!$AH9</f>
         <v>19.773137501487192</v>
       </c>
-      <c r="S8">
+      <c r="R8">
         <f>'[1]Formula (ppm) Duplicates Remove'!S9*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG9))/'[1]Formula (ppm) Duplicates Remove'!$AH9</f>
         <v>164.04258569215219</v>
       </c>
-      <c r="T8">
+      <c r="S8">
         <f>'[1]Formula (ppm) Duplicates Remove'!T9*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG9))/'[1]Formula (ppm) Duplicates Remove'!$AH9</f>
         <v>5.3815355163723479</v>
       </c>
-      <c r="U8">
+      <c r="T8">
         <f>'[1]Formula (ppm) Duplicates Remove'!U9*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG9))/'[1]Formula (ppm) Duplicates Remove'!$AH9</f>
         <v>23.948304285642969</v>
       </c>
-      <c r="V8">
+      <c r="U8">
         <f>'[1]Formula (ppm) Duplicates Remove'!V9*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG9))/'[1]Formula (ppm) Duplicates Remove'!$AH9</f>
         <v>5.4003850278132308</v>
       </c>
-      <c r="W8">
+      <c r="V8">
         <f>'[1]Formula (ppm) Duplicates Remove'!W9*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG9))/'[1]Formula (ppm) Duplicates Remove'!$AH9</f>
         <v>1.1121211750121489</v>
       </c>
-      <c r="X8">
+      <c r="W8">
         <f>'[1]Formula (ppm) Duplicates Remove'!X9*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG9))/'[1]Formula (ppm) Duplicates Remove'!$AH9</f>
         <v>6.2815996876745528</v>
       </c>
-      <c r="Y8">
+      <c r="X8">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y9*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG9))/'[1]Formula (ppm) Duplicates Remove'!$AH9</f>
         <v>4.4107856771668281</v>
       </c>
-      <c r="Z8">
+      <c r="Y8">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z9*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG9))/'[1]Formula (ppm) Duplicates Remove'!$AH9</f>
         <v>1.0320107513883925</v>
       </c>
-      <c r="AA8">
+      <c r="Z8">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA9*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG9))/'[1]Formula (ppm) Duplicates Remove'!$AH9</f>
         <v>2.1252824149596576</v>
       </c>
-      <c r="AB8">
+      <c r="AA8">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB9*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG9))/'[1]Formula (ppm) Duplicates Remove'!$AH9</f>
         <v>0.26860553803259529</v>
       </c>
-      <c r="AC8">
+      <c r="AB8">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC9*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG9))/'[1]Formula (ppm) Duplicates Remove'!$AH9</f>
         <v>1.5974960946149088</v>
       </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
       <c r="AD8">
-        <v>0</v>
-      </c>
-      <c r="AE8">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE9*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG9))/'[1]Formula (ppm) Duplicates Remove'!$AH9</f>
         <v>9.0289159801833776</v>
       </c>
-      <c r="AF8">
+      <c r="AE8">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF9*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG9))/'[1]Formula (ppm) Duplicates Remove'!$AH9</f>
         <v>3.1997045670900386</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -4219,73 +4191,70 @@
         <v>274.14264412729756</v>
       </c>
       <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q10*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG10))/'[1]Formula (ppm) Duplicates Remove'!$AH10</f>
         <v>75.589222464068484</v>
       </c>
-      <c r="R9">
+      <c r="Q9">
         <f>'[1]Formula (ppm) Duplicates Remove'!R10*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG10))/'[1]Formula (ppm) Duplicates Remove'!$AH10</f>
         <v>20.297619531804159</v>
       </c>
-      <c r="S9">
+      <c r="R9">
         <f>'[1]Formula (ppm) Duplicates Remove'!S10*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG10))/'[1]Formula (ppm) Duplicates Remove'!$AH10</f>
         <v>150.80410358431274</v>
       </c>
-      <c r="T9">
+      <c r="S9">
         <f>'[1]Formula (ppm) Duplicates Remove'!T10*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG10))/'[1]Formula (ppm) Duplicates Remove'!$AH10</f>
         <v>3.9860420870175512</v>
       </c>
-      <c r="U9">
+      <c r="T9">
         <f>'[1]Formula (ppm) Duplicates Remove'!U10*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG10))/'[1]Formula (ppm) Duplicates Remove'!$AH10</f>
         <v>15.264808131500258</v>
       </c>
-      <c r="V9">
+      <c r="U9">
         <f>'[1]Formula (ppm) Duplicates Remove'!V10*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG10))/'[1]Formula (ppm) Duplicates Remove'!$AH10</f>
         <v>2.9462050208390598</v>
       </c>
-      <c r="W9">
+      <c r="V9">
         <f>'[1]Formula (ppm) Duplicates Remove'!W10*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG10))/'[1]Formula (ppm) Duplicates Remove'!$AH10</f>
         <v>0.56151201573638554</v>
       </c>
-      <c r="X9">
+      <c r="W9">
         <f>'[1]Formula (ppm) Duplicates Remove'!X10*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG10))/'[1]Formula (ppm) Duplicates Remove'!$AH10</f>
         <v>3.521581530791158</v>
       </c>
-      <c r="Y9">
+      <c r="X9">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y10*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG10))/'[1]Formula (ppm) Duplicates Remove'!$AH10</f>
         <v>2.0727418852491266</v>
       </c>
-      <c r="Z9">
+      <c r="Y9">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z10*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG10))/'[1]Formula (ppm) Duplicates Remove'!$AH10</f>
         <v>0.47139280333424954</v>
       </c>
-      <c r="AA9">
+      <c r="Z9">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA10*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG10))/'[1]Formula (ppm) Duplicates Remove'!$AH10</f>
         <v>1.2408722323063333</v>
       </c>
-      <c r="AB9">
+      <c r="AA9">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB10*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG10))/'[1]Formula (ppm) Duplicates Remove'!$AH10</f>
         <v>0.17330617769641526</v>
       </c>
-      <c r="AC9">
+      <c r="AB9">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC10*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG10))/'[1]Formula (ppm) Duplicates Remove'!$AH10</f>
         <v>1.143820772796341</v>
       </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
       <c r="AD9">
-        <v>0</v>
-      </c>
-      <c r="AE9">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE10*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG10))/'[1]Formula (ppm) Duplicates Remove'!$AH10</f>
         <v>15.895642618315211</v>
       </c>
-      <c r="AF9">
+      <c r="AE9">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF10*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG10))/'[1]Formula (ppm) Duplicates Remove'!$AH10</f>
         <v>0.67936021656994794</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -4346,73 +4315,70 @@
         <v>261.52183286712949</v>
       </c>
       <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q11*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG11))/'[1]Formula (ppm) Duplicates Remove'!$AH11</f>
         <v>112.8830435662484</v>
       </c>
-      <c r="R10">
+      <c r="Q10">
         <f>'[1]Formula (ppm) Duplicates Remove'!R11*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG11))/'[1]Formula (ppm) Duplicates Remove'!$AH11</f>
         <v>18.514820025991469</v>
       </c>
-      <c r="S10">
+      <c r="R10">
         <f>'[1]Formula (ppm) Duplicates Remove'!S11*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG11))/'[1]Formula (ppm) Duplicates Remove'!$AH11</f>
         <v>246.38850194530869</v>
       </c>
-      <c r="T10">
+      <c r="S10">
         <f>'[1]Formula (ppm) Duplicates Remove'!T11*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG11))/'[1]Formula (ppm) Duplicates Remove'!$AH11</f>
         <v>4.728749062834277</v>
       </c>
-      <c r="U10">
+      <c r="T10">
         <f>'[1]Formula (ppm) Duplicates Remove'!U11*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG11))/'[1]Formula (ppm) Duplicates Remove'!$AH11</f>
         <v>19.228467627857857</v>
       </c>
-      <c r="V10">
+      <c r="U10">
         <f>'[1]Formula (ppm) Duplicates Remove'!V11*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG11))/'[1]Formula (ppm) Duplicates Remove'!$AH11</f>
         <v>3.7883349332720293</v>
       </c>
-      <c r="W10">
+      <c r="V10">
         <f>'[1]Formula (ppm) Duplicates Remove'!W11*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG11))/'[1]Formula (ppm) Duplicates Remove'!$AH11</f>
         <v>0.79368284693551316</v>
       </c>
-      <c r="X10">
+      <c r="W10">
         <f>'[1]Formula (ppm) Duplicates Remove'!X11*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG11))/'[1]Formula (ppm) Duplicates Remove'!$AH11</f>
         <v>5.0555596468665467</v>
       </c>
-      <c r="Y10">
+      <c r="X10">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y11*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG11))/'[1]Formula (ppm) Duplicates Remove'!$AH11</f>
         <v>2.1009251830645943</v>
       </c>
-      <c r="Z10">
+      <c r="Y10">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z11*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG11))/'[1]Formula (ppm) Duplicates Remove'!$AH11</f>
         <v>0.39350662158987637</v>
       </c>
-      <c r="AA10">
+      <c r="Z10">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA11*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG11))/'[1]Formula (ppm) Duplicates Remove'!$AH11</f>
         <v>0.95375333707376797</v>
       </c>
-      <c r="AB10">
+      <c r="AA10">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB11*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG11))/'[1]Formula (ppm) Duplicates Remove'!$AH11</f>
         <v>0.10671366009216984</v>
       </c>
-      <c r="AC10">
+      <c r="AB10">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC11*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG11))/'[1]Formula (ppm) Duplicates Remove'!$AH11</f>
         <v>0.62027314928573729</v>
       </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
       <c r="AD10">
-        <v>0</v>
-      </c>
-      <c r="AE10">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE11*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG11))/'[1]Formula (ppm) Duplicates Remove'!$AH11</f>
         <v>30.526776390116343</v>
       </c>
-      <c r="AF10">
+      <c r="AE10">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF11*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG11))/'[1]Formula (ppm) Duplicates Remove'!$AH11</f>
         <v>2.9613040675577138</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -4473,73 +4439,70 @@
         <v>2.2761614577326905</v>
       </c>
       <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q12*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG12))/'[1]Formula (ppm) Duplicates Remove'!$AH12</f>
         <v>660.68142731629734</v>
       </c>
-      <c r="R11">
+      <c r="Q11">
         <f>'[1]Formula (ppm) Duplicates Remove'!R12*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG12))/'[1]Formula (ppm) Duplicates Remove'!$AH12</f>
         <v>63.694647913724459</v>
       </c>
-      <c r="S11">
+      <c r="R11">
         <f>'[1]Formula (ppm) Duplicates Remove'!S12*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG12))/'[1]Formula (ppm) Duplicates Remove'!$AH12</f>
         <v>731.75371669368781</v>
       </c>
-      <c r="T11">
+      <c r="S11">
         <f>'[1]Formula (ppm) Duplicates Remove'!T12*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG12))/'[1]Formula (ppm) Duplicates Remove'!$AH12</f>
         <v>14.012974032630542</v>
       </c>
-      <c r="U11">
+      <c r="T11">
         <f>'[1]Formula (ppm) Duplicates Remove'!U12*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG12))/'[1]Formula (ppm) Duplicates Remove'!$AH12</f>
         <v>52.942530811389815</v>
       </c>
-      <c r="V11">
+      <c r="U11">
         <f>'[1]Formula (ppm) Duplicates Remove'!V12*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG12))/'[1]Formula (ppm) Duplicates Remove'!$AH12</f>
         <v>9.070560218418958</v>
       </c>
-      <c r="W11">
+      <c r="V11">
         <f>'[1]Formula (ppm) Duplicates Remove'!W12*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG12))/'[1]Formula (ppm) Duplicates Remove'!$AH12</f>
         <v>1.7648772700556306</v>
       </c>
-      <c r="X11">
+      <c r="W11">
         <f>'[1]Formula (ppm) Duplicates Remove'!X12*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG12))/'[1]Formula (ppm) Duplicates Remove'!$AH12</f>
         <v>11.710301542944228</v>
       </c>
-      <c r="Y11">
+      <c r="X11">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y12*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG12))/'[1]Formula (ppm) Duplicates Remove'!$AH12</f>
         <v>5.1090545864915136</v>
       </c>
-      <c r="Z11">
+      <c r="Y11">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z12*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG12))/'[1]Formula (ppm) Duplicates Remove'!$AH12</f>
         <v>1.1021014712149966</v>
       </c>
-      <c r="AA11">
+      <c r="Z11">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA12*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG12))/'[1]Formula (ppm) Duplicates Remove'!$AH12</f>
         <v>2.6397413245252666</v>
       </c>
-      <c r="AB11">
+      <c r="AA11">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB12*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG12))/'[1]Formula (ppm) Duplicates Remove'!$AH12</f>
         <v>0.35600528623439748</v>
       </c>
-      <c r="AC11">
+      <c r="AB11">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC12*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG12))/'[1]Formula (ppm) Duplicates Remove'!$AH12</f>
         <v>2.1928410715927251</v>
       </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
       <c r="AD11">
-        <v>0</v>
-      </c>
-      <c r="AE11">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE12*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG12))/'[1]Formula (ppm) Duplicates Remove'!$AH12</f>
         <v>22.651783159233318</v>
       </c>
-      <c r="AF11">
+      <c r="AE11">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF12*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG12))/'[1]Formula (ppm) Duplicates Remove'!$AH12</f>
         <v>2.3216089410817626</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -4600,73 +4563,70 @@
         <v>8.0222453317060438</v>
       </c>
       <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q13*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG13))/'[1]Formula (ppm) Duplicates Remove'!$AH13</f>
         <v>881.64097532487017</v>
       </c>
-      <c r="R12">
+      <c r="Q12">
         <f>'[1]Formula (ppm) Duplicates Remove'!R13*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG13))/'[1]Formula (ppm) Duplicates Remove'!$AH13</f>
         <v>56.610112876806298</v>
       </c>
-      <c r="S12">
+      <c r="R12">
         <f>'[1]Formula (ppm) Duplicates Remove'!S13*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG13))/'[1]Formula (ppm) Duplicates Remove'!$AH13</f>
         <v>461.7957110432107</v>
       </c>
-      <c r="T12">
+      <c r="S12">
         <f>'[1]Formula (ppm) Duplicates Remove'!T13*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG13))/'[1]Formula (ppm) Duplicates Remove'!$AH13</f>
         <v>13.036824847883727</v>
       </c>
-      <c r="U12">
+      <c r="T12">
         <f>'[1]Formula (ppm) Duplicates Remove'!U13*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG13))/'[1]Formula (ppm) Duplicates Remove'!$AH13</f>
         <v>50.946396853680049</v>
       </c>
-      <c r="V12">
+      <c r="U12">
         <f>'[1]Formula (ppm) Duplicates Remove'!V13*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG13))/'[1]Formula (ppm) Duplicates Remove'!$AH13</f>
         <v>9.4503456469928917</v>
       </c>
-      <c r="W12">
+      <c r="V12">
         <f>'[1]Formula (ppm) Duplicates Remove'!W13*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG13))/'[1]Formula (ppm) Duplicates Remove'!$AH13</f>
         <v>2.0339610551055105</v>
       </c>
-      <c r="X12">
+      <c r="W12">
         <f>'[1]Formula (ppm) Duplicates Remove'!X13*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG13))/'[1]Formula (ppm) Duplicates Remove'!$AH13</f>
         <v>11.084005856146787</v>
       </c>
-      <c r="Y12">
+      <c r="X12">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y13*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG13))/'[1]Formula (ppm) Duplicates Remove'!$AH13</f>
         <v>6.1938441704675791</v>
       </c>
-      <c r="Z12">
+      <c r="Y12">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z13*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG13))/'[1]Formula (ppm) Duplicates Remove'!$AH13</f>
         <v>1.3794150772657054</v>
       </c>
-      <c r="AA12">
+      <c r="Z12">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA13*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG13))/'[1]Formula (ppm) Duplicates Remove'!$AH13</f>
         <v>3.1266741751355989</v>
       </c>
-      <c r="AB12">
+      <c r="AA12">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB13*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG13))/'[1]Formula (ppm) Duplicates Remove'!$AH13</f>
         <v>0.38948190416914025</v>
       </c>
-      <c r="AC12">
+      <c r="AB12">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC13*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG13))/'[1]Formula (ppm) Duplicates Remove'!$AH13</f>
         <v>2.4126240174921745</v>
       </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
       <c r="AD12">
-        <v>0</v>
-      </c>
-      <c r="AE12">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE13*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG13))/'[1]Formula (ppm) Duplicates Remove'!$AH13</f>
         <v>42.085683533832118</v>
       </c>
-      <c r="AF12">
+      <c r="AE12">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF13*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG13))/'[1]Formula (ppm) Duplicates Remove'!$AH13</f>
         <v>1.6066128546977039</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -4727,73 +4687,70 @@
         <v>16.86393330783028</v>
       </c>
       <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q14*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG14))/'[1]Formula (ppm) Duplicates Remove'!$AH14</f>
         <v>18.087098308972724</v>
       </c>
-      <c r="R13">
+      <c r="Q13">
         <f>'[1]Formula (ppm) Duplicates Remove'!R14*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG14))/'[1]Formula (ppm) Duplicates Remove'!$AH14</f>
         <v>3.8208768104994277</v>
       </c>
-      <c r="S13">
+      <c r="R13">
         <f>'[1]Formula (ppm) Duplicates Remove'!S14*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG14))/'[1]Formula (ppm) Duplicates Remove'!$AH14</f>
         <v>16.234184990410405</v>
       </c>
-      <c r="T13">
+      <c r="S13">
         <f>'[1]Formula (ppm) Duplicates Remove'!T14*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG14))/'[1]Formula (ppm) Duplicates Remove'!$AH14</f>
         <v>1.0596726495045956</v>
       </c>
-      <c r="U13">
+      <c r="T13">
         <f>'[1]Formula (ppm) Duplicates Remove'!U14*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG14))/'[1]Formula (ppm) Duplicates Remove'!$AH14</f>
         <v>4.5838411181427361</v>
       </c>
-      <c r="V13">
+      <c r="U13">
         <f>'[1]Formula (ppm) Duplicates Remove'!V14*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG14))/'[1]Formula (ppm) Duplicates Remove'!$AH14</f>
         <v>0.93856720384692749</v>
       </c>
-      <c r="W13">
+      <c r="V13">
         <f>'[1]Formula (ppm) Duplicates Remove'!W14*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG14))/'[1]Formula (ppm) Duplicates Remove'!$AH14</f>
         <v>0.21193452990091913</v>
       </c>
-      <c r="X13">
+      <c r="W13">
         <f>'[1]Formula (ppm) Duplicates Remove'!X14*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG14))/'[1]Formula (ppm) Duplicates Remove'!$AH14</f>
         <v>1.0475621049388284</v>
       </c>
-      <c r="Y13">
+      <c r="X13">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y14*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG14))/'[1]Formula (ppm) Duplicates Remove'!$AH14</f>
         <v>0.79324066905772583</v>
       </c>
-      <c r="Z13">
+      <c r="Y13">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z14*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG14))/'[1]Formula (ppm) Duplicates Remove'!$AH14</f>
         <v>0.19376871305226886</v>
       </c>
-      <c r="AA13">
+      <c r="Z13">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA14*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG14))/'[1]Formula (ppm) Duplicates Remove'!$AH14</f>
         <v>0.42992433208472158</v>
       </c>
-      <c r="AB13">
+      <c r="AA13">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB14*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG14))/'[1]Formula (ppm) Duplicates Remove'!$AH14</f>
         <v>4.8442178263067216E-2</v>
       </c>
-      <c r="AC13">
+      <c r="AB13">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC14*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG14))/'[1]Formula (ppm) Duplicates Remove'!$AH14</f>
         <v>0.30276361414417013</v>
       </c>
+      <c r="AC13">
+        <v>0</v>
+      </c>
       <c r="AD13">
-        <v>0</v>
-      </c>
-      <c r="AE13">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE14*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG14))/'[1]Formula (ppm) Duplicates Remove'!$AH14</f>
         <v>2.6340434430542801</v>
       </c>
-      <c r="AF13">
+      <c r="AE13">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF14*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG14))/'[1]Formula (ppm) Duplicates Remove'!$AH14</f>
         <v>0.35120579240723737</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -4854,73 +4811,70 @@
         <v>6.7216114649849663</v>
       </c>
       <c r="P14">
-        <v>0</v>
-      </c>
-      <c r="Q14">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q15*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG15))/'[1]Formula (ppm) Duplicates Remove'!$AH15</f>
         <v>612.04776561319295</v>
       </c>
-      <c r="R14">
+      <c r="Q14">
         <f>'[1]Formula (ppm) Duplicates Remove'!R15*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG15))/'[1]Formula (ppm) Duplicates Remove'!$AH15</f>
         <v>11.862431573836226</v>
       </c>
-      <c r="S14">
+      <c r="R14">
         <f>'[1]Formula (ppm) Duplicates Remove'!S15*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG15))/'[1]Formula (ppm) Duplicates Remove'!$AH15</f>
         <v>69.801682977553284</v>
       </c>
-      <c r="T14">
+      <c r="S14">
         <f>'[1]Formula (ppm) Duplicates Remove'!T15*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG15))/'[1]Formula (ppm) Duplicates Remove'!$AH15</f>
         <v>2.4253237244791119</v>
       </c>
-      <c r="U14">
+      <c r="T14">
         <f>'[1]Formula (ppm) Duplicates Remove'!U15*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG15))/'[1]Formula (ppm) Duplicates Remove'!$AH15</f>
         <v>9.7749207966952785</v>
       </c>
-      <c r="V14">
+      <c r="U14">
         <f>'[1]Formula (ppm) Duplicates Remove'!V15*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG15))/'[1]Formula (ppm) Duplicates Remove'!$AH15</f>
         <v>1.9489208500278574</v>
       </c>
-      <c r="W14">
+      <c r="V14">
         <f>'[1]Formula (ppm) Duplicates Remove'!W15*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG15))/'[1]Formula (ppm) Duplicates Remove'!$AH15</f>
         <v>0.55002877323008426</v>
       </c>
-      <c r="X14">
+      <c r="W14">
         <f>'[1]Formula (ppm) Duplicates Remove'!X15*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG15))/'[1]Formula (ppm) Duplicates Remove'!$AH15</f>
         <v>2.4902877528133733</v>
       </c>
-      <c r="Y14">
+      <c r="X14">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y15*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG15))/'[1]Formula (ppm) Duplicates Remove'!$AH15</f>
         <v>1.68906473669081</v>
       </c>
-      <c r="Z14">
+      <c r="Y14">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z15*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG15))/'[1]Formula (ppm) Duplicates Remove'!$AH15</f>
         <v>0.41143884611699216</v>
       </c>
-      <c r="AA14">
+      <c r="Z14">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA15*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG15))/'[1]Formula (ppm) Duplicates Remove'!$AH15</f>
         <v>0.94847481368022413</v>
       </c>
-      <c r="AB14">
+      <c r="AA14">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB15*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG15))/'[1]Formula (ppm) Duplicates Remove'!$AH15</f>
         <v>0.13425899189080798</v>
       </c>
-      <c r="AC14">
+      <c r="AB14">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC15*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG15))/'[1]Formula (ppm) Duplicates Remove'!$AH15</f>
         <v>0.70594244123231287</v>
       </c>
+      <c r="AC14">
+        <v>0</v>
+      </c>
       <c r="AD14">
-        <v>0</v>
-      </c>
-      <c r="AE14">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE15*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG15))/'[1]Formula (ppm) Duplicates Remove'!$AH15</f>
         <v>15.292532269885257</v>
       </c>
-      <c r="AF14">
+      <c r="AE14">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF15*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG15))/'[1]Formula (ppm) Duplicates Remove'!$AH15</f>
         <v>0.92682013756880333</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -4981,73 +4935,70 @@
         <v>1.1455230064243487</v>
       </c>
       <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q16*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG16))/'[1]Formula (ppm) Duplicates Remove'!$AH16</f>
         <v>2080.4648962226565</v>
       </c>
-      <c r="R15">
+      <c r="Q15">
         <f>'[1]Formula (ppm) Duplicates Remove'!R16*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG16))/'[1]Formula (ppm) Duplicates Remove'!$AH16</f>
         <v>4.7520322519251827</v>
       </c>
-      <c r="S15">
+      <c r="R15">
         <f>'[1]Formula (ppm) Duplicates Remove'!S16*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG16))/'[1]Formula (ppm) Duplicates Remove'!$AH16</f>
         <v>7.1311954191142153</v>
       </c>
-      <c r="T15">
+      <c r="S15">
         <f>'[1]Formula (ppm) Duplicates Remove'!T16*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG16))/'[1]Formula (ppm) Duplicates Remove'!$AH16</f>
         <v>1.019641357366728</v>
       </c>
-      <c r="U15">
+      <c r="T15">
         <f>'[1]Formula (ppm) Duplicates Remove'!U16*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG16))/'[1]Formula (ppm) Duplicates Remove'!$AH16</f>
         <v>4.1289180890899599</v>
       </c>
-      <c r="V15">
+      <c r="U15">
         <f>'[1]Formula (ppm) Duplicates Remove'!V16*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG16))/'[1]Formula (ppm) Duplicates Remove'!$AH16</f>
         <v>0.87487746095046415</v>
       </c>
-      <c r="W15">
+      <c r="V15">
         <f>'[1]Formula (ppm) Duplicates Remove'!W16*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG16))/'[1]Formula (ppm) Duplicates Remove'!$AH16</f>
         <v>0.64829049264674665</v>
       </c>
-      <c r="X15">
+      <c r="W15">
         <f>'[1]Formula (ppm) Duplicates Remove'!X16*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG16))/'[1]Formula (ppm) Duplicates Remove'!$AH16</f>
         <v>0.81193663642165359</v>
       </c>
-      <c r="Y15">
+      <c r="X15">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y16*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG16))/'[1]Formula (ppm) Duplicates Remove'!$AH16</f>
         <v>0.64829049264674665</v>
       </c>
-      <c r="Z15">
+      <c r="Y15">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z16*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG16))/'[1]Formula (ppm) Duplicates Remove'!$AH16</f>
         <v>0.17623430868066903</v>
       </c>
-      <c r="AA15">
+      <c r="Z15">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA16*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG16))/'[1]Formula (ppm) Duplicates Remove'!$AH16</f>
         <v>0.42170352434302943</v>
       </c>
-      <c r="AB15">
+      <c r="AA15">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB16*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG16))/'[1]Formula (ppm) Duplicates Remove'!$AH16</f>
         <v>5.0352659623048288E-2</v>
       </c>
-      <c r="AC15">
+      <c r="AB15">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC16*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG16))/'[1]Formula (ppm) Duplicates Remove'!$AH16</f>
         <v>0.31470412264405184</v>
       </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
       <c r="AD15">
-        <v>0</v>
-      </c>
-      <c r="AE15">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE16*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG16))/'[1]Formula (ppm) Duplicates Remove'!$AH16</f>
         <v>2.0078123024690506</v>
       </c>
-      <c r="AF15">
+      <c r="AE15">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF16*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG16))/'[1]Formula (ppm) Duplicates Remove'!$AH16</f>
         <v>2.265869683037173</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -5108,73 +5059,70 @@
         <v>2.2653838468018952</v>
       </c>
       <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="Q16">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q17*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG17))/'[1]Formula (ppm) Duplicates Remove'!$AH17</f>
         <v>25519.723294519255</v>
       </c>
-      <c r="R16">
+      <c r="Q16">
         <f>'[1]Formula (ppm) Duplicates Remove'!R17*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG17))/'[1]Formula (ppm) Duplicates Remove'!$AH17</f>
         <v>4.8177846515696405</v>
       </c>
-      <c r="S16">
+      <c r="R16">
         <f>'[1]Formula (ppm) Duplicates Remove'!S17*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG17))/'[1]Formula (ppm) Duplicates Remove'!$AH17</f>
         <v>6.8269033573305977</v>
       </c>
-      <c r="T16">
+      <c r="S16">
         <f>'[1]Formula (ppm) Duplicates Remove'!T17*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG17))/'[1]Formula (ppm) Duplicates Remove'!$AH17</f>
         <v>1.0250605641637534</v>
       </c>
-      <c r="U16">
+      <c r="T16">
         <f>'[1]Formula (ppm) Duplicates Remove'!U17*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG17))/'[1]Formula (ppm) Duplicates Remove'!$AH17</f>
         <v>4.2027483130713881</v>
       </c>
-      <c r="V16">
+      <c r="U16">
         <f>'[1]Formula (ppm) Duplicates Remove'!V17*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG17))/'[1]Formula (ppm) Duplicates Remove'!$AH17</f>
         <v>0.87130147953919057</v>
       </c>
-      <c r="W16">
+      <c r="V16">
         <f>'[1]Formula (ppm) Duplicates Remove'!W17*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG17))/'[1]Formula (ppm) Duplicates Remove'!$AH17</f>
         <v>6.0478573285661437</v>
       </c>
-      <c r="X16">
+      <c r="W16">
         <f>'[1]Formula (ppm) Duplicates Remove'!X17*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG17))/'[1]Formula (ppm) Duplicates Remove'!$AH17</f>
         <v>0.93280511338901562</v>
       </c>
-      <c r="Y16">
+      <c r="X16">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y17*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG17))/'[1]Formula (ppm) Duplicates Remove'!$AH17</f>
         <v>0.53303149336515177</v>
       </c>
-      <c r="Z16">
+      <c r="Y16">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z17*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG17))/'[1]Formula (ppm) Duplicates Remove'!$AH17</f>
         <v>0.14350847898292549</v>
       </c>
-      <c r="AA16">
+      <c r="Z16">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA17*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG17))/'[1]Formula (ppm) Duplicates Remove'!$AH17</f>
         <v>0.27676635232421343</v>
       </c>
-      <c r="AB16">
+      <c r="AA16">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB17*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG17))/'[1]Formula (ppm) Duplicates Remove'!$AH17</f>
         <v>4.1002422566550137E-2</v>
       </c>
-      <c r="AC16">
+      <c r="AB16">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC17*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG17))/'[1]Formula (ppm) Duplicates Remove'!$AH17</f>
         <v>0.24601453539930079</v>
       </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
       <c r="AD16">
-        <v>0</v>
-      </c>
-      <c r="AE16">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE17*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG17))/'[1]Formula (ppm) Duplicates Remove'!$AH17</f>
         <v>4.6947773838699911</v>
       </c>
-      <c r="AF16">
+      <c r="AE16">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF17*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG17))/'[1]Formula (ppm) Duplicates Remove'!$AH17</f>
         <v>2.0808729452524193</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -5235,73 +5183,70 @@
         <v>10.9960592489745</v>
       </c>
       <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q18*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG18))/'[1]Formula (ppm) Duplicates Remove'!$AH18</f>
         <v>170.56319182684453</v>
       </c>
-      <c r="R17">
+      <c r="Q17">
         <f>'[1]Formula (ppm) Duplicates Remove'!R18*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG18))/'[1]Formula (ppm) Duplicates Remove'!$AH18</f>
         <v>6.247955722916922</v>
       </c>
-      <c r="S17">
+      <c r="R17">
         <f>'[1]Formula (ppm) Duplicates Remove'!S18*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG18))/'[1]Formula (ppm) Duplicates Remove'!$AH18</f>
         <v>43.898531156077468</v>
       </c>
-      <c r="T17">
+      <c r="S17">
         <f>'[1]Formula (ppm) Duplicates Remove'!T18*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG18))/'[1]Formula (ppm) Duplicates Remove'!$AH18</f>
         <v>1.43985810898497</v>
       </c>
-      <c r="U17">
+      <c r="T17">
         <f>'[1]Formula (ppm) Duplicates Remove'!U18*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG18))/'[1]Formula (ppm) Duplicates Remove'!$AH18</f>
         <v>6.3465174387105368</v>
       </c>
-      <c r="V17">
+      <c r="U17">
         <f>'[1]Formula (ppm) Duplicates Remove'!V18*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG18))/'[1]Formula (ppm) Duplicates Remove'!$AH18</f>
         <v>1.3498669771734093</v>
       </c>
-      <c r="W17">
+      <c r="V17">
         <f>'[1]Formula (ppm) Duplicates Remove'!W18*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG18))/'[1]Formula (ppm) Duplicates Remove'!$AH18</f>
         <v>0.32139689932700216</v>
       </c>
-      <c r="X17">
+      <c r="W17">
         <f>'[1]Formula (ppm) Duplicates Remove'!X18*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG18))/'[1]Formula (ppm) Duplicates Remove'!$AH18</f>
         <v>1.7398285483568385</v>
       </c>
-      <c r="Y17">
+      <c r="X17">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y18*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG18))/'[1]Formula (ppm) Duplicates Remove'!$AH18</f>
         <v>1.4227169410208629</v>
       </c>
-      <c r="Z17">
+      <c r="Y17">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z18*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG18))/'[1]Formula (ppm) Duplicates Remove'!$AH18</f>
         <v>0.38567627919240255</v>
       </c>
-      <c r="AA17">
+      <c r="Z17">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA18*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG18))/'[1]Formula (ppm) Duplicates Remove'!$AH18</f>
         <v>0.86562898218739248</v>
       </c>
-      <c r="AB17">
+      <c r="AA17">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB18*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG18))/'[1]Formula (ppm) Duplicates Remove'!$AH18</f>
         <v>0.10713229977566739</v>
       </c>
-      <c r="AC17">
+      <c r="AB17">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC18*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG18))/'[1]Formula (ppm) Duplicates Remove'!$AH18</f>
         <v>0.62993792268092419</v>
       </c>
+      <c r="AC17">
+        <v>0</v>
+      </c>
       <c r="AD17">
-        <v>0</v>
-      </c>
-      <c r="AE17">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE18*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG18))/'[1]Formula (ppm) Duplicates Remove'!$AH18</f>
         <v>8.5105898941790166</v>
       </c>
-      <c r="AF17">
+      <c r="AE17">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF18*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG18))/'[1]Formula (ppm) Duplicates Remove'!$AH18</f>
         <v>0.50566445494115009</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -5362,73 +5307,70 @@
         <v>11.772411483849247</v>
       </c>
       <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q19*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG19))/'[1]Formula (ppm) Duplicates Remove'!$AH19</f>
         <v>55.563552228428172</v>
       </c>
-      <c r="R18">
+      <c r="Q18">
         <f>'[1]Formula (ppm) Duplicates Remove'!R19*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG19))/'[1]Formula (ppm) Duplicates Remove'!$AH19</f>
         <v>2.8757390325582808</v>
       </c>
-      <c r="S18">
+      <c r="R18">
         <f>'[1]Formula (ppm) Duplicates Remove'!S19*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG19))/'[1]Formula (ppm) Duplicates Remove'!$AH19</f>
         <v>16.729460833994136</v>
       </c>
-      <c r="T18">
+      <c r="S18">
         <f>'[1]Formula (ppm) Duplicates Remove'!T19*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG19))/'[1]Formula (ppm) Duplicates Remove'!$AH19</f>
         <v>0.71080463971149754</v>
       </c>
-      <c r="U18">
+      <c r="T18">
         <f>'[1]Formula (ppm) Duplicates Remove'!U19*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG19))/'[1]Formula (ppm) Duplicates Remove'!$AH19</f>
         <v>2.8525101227637872</v>
       </c>
-      <c r="V18">
+      <c r="U18">
         <f>'[1]Formula (ppm) Duplicates Remove'!V19*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG19))/'[1]Formula (ppm) Duplicates Remove'!$AH19</f>
         <v>0.54355648919114519</v>
       </c>
-      <c r="W18">
+      <c r="V18">
         <f>'[1]Formula (ppm) Duplicates Remove'!W19*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG19))/'[1]Formula (ppm) Duplicates Remove'!$AH19</f>
         <v>0.11614454897246693</v>
       </c>
-      <c r="X18">
+      <c r="W18">
         <f>'[1]Formula (ppm) Duplicates Remove'!X19*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG19))/'[1]Formula (ppm) Duplicates Remove'!$AH19</f>
         <v>0.66899260208140943</v>
       </c>
-      <c r="Y18">
+      <c r="X18">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y19*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG19))/'[1]Formula (ppm) Duplicates Remove'!$AH19</f>
         <v>0.43670350413647563</v>
       </c>
-      <c r="Z18">
+      <c r="Y18">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z19*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG19))/'[1]Formula (ppm) Duplicates Remove'!$AH19</f>
         <v>0.10220720309577087</v>
       </c>
-      <c r="AA18">
+      <c r="Z18">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA19*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG19))/'[1]Formula (ppm) Duplicates Remove'!$AH19</f>
         <v>0.24158066186273119</v>
       </c>
-      <c r="AB18">
+      <c r="AA18">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB19*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG19))/'[1]Formula (ppm) Duplicates Remove'!$AH19</f>
         <v>3.2520473712290741E-2</v>
       </c>
-      <c r="AC18">
+      <c r="AB18">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC19*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG19))/'[1]Formula (ppm) Duplicates Remove'!$AH19</f>
         <v>0.19976862423264308</v>
       </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
       <c r="AD18">
-        <v>0</v>
-      </c>
-      <c r="AE18">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE19*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG19))/'[1]Formula (ppm) Duplicates Remove'!$AH19</f>
         <v>6.5319694342115397</v>
       </c>
-      <c r="AF18">
+      <c r="AE18">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF19*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG19))/'[1]Formula (ppm) Duplicates Remove'!$AH19</f>
         <v>0.25551800773942723</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -5489,73 +5431,70 @@
         <v>11.038549891107415</v>
       </c>
       <c r="P19">
-        <v>0</v>
-      </c>
-      <c r="Q19">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q20*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG20))/'[1]Formula (ppm) Duplicates Remove'!$AH20</f>
         <v>37.164607649574599</v>
       </c>
-      <c r="R19">
+      <c r="Q19">
         <f>'[1]Formula (ppm) Duplicates Remove'!R20*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG20))/'[1]Formula (ppm) Duplicates Remove'!$AH20</f>
         <v>6.417553701874593</v>
       </c>
-      <c r="S19">
+      <c r="R19">
         <f>'[1]Formula (ppm) Duplicates Remove'!S20*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG20))/'[1]Formula (ppm) Duplicates Remove'!$AH20</f>
         <v>67.277056704749398</v>
       </c>
-      <c r="T19">
+      <c r="S19">
         <f>'[1]Formula (ppm) Duplicates Remove'!T20*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG20))/'[1]Formula (ppm) Duplicates Remove'!$AH20</f>
         <v>1.3407145616729652</v>
       </c>
-      <c r="U19">
+      <c r="T19">
         <f>'[1]Formula (ppm) Duplicates Remove'!U20*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG20))/'[1]Formula (ppm) Duplicates Remove'!$AH20</f>
         <v>5.3449820525362215</v>
       </c>
-      <c r="V19">
+      <c r="U19">
         <f>'[1]Formula (ppm) Duplicates Remove'!V20*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG20))/'[1]Formula (ppm) Duplicates Remove'!$AH20</f>
         <v>0.99659782417690423</v>
       </c>
-      <c r="W19">
+      <c r="V19">
         <f>'[1]Formula (ppm) Duplicates Remove'!W20*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG20))/'[1]Formula (ppm) Duplicates Remove'!$AH20</f>
         <v>0.20110718425094476</v>
       </c>
-      <c r="X19">
+      <c r="W19">
         <f>'[1]Formula (ppm) Duplicates Remove'!X20*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG20))/'[1]Formula (ppm) Duplicates Remove'!$AH20</f>
         <v>1.3496526587507849</v>
       </c>
-      <c r="Y19">
+      <c r="X19">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y20*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG20))/'[1]Formula (ppm) Duplicates Remove'!$AH20</f>
         <v>0.78655254284813958</v>
       </c>
-      <c r="Z19">
+      <c r="Y19">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z20*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG20))/'[1]Formula (ppm) Duplicates Remove'!$AH20</f>
         <v>0.20557623278985468</v>
       </c>
-      <c r="AA19">
+      <c r="Z19">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA20*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG20))/'[1]Formula (ppm) Duplicates Remove'!$AH20</f>
         <v>0.46925009658553785</v>
       </c>
-      <c r="AB19">
+      <c r="AA19">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB20*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG20))/'[1]Formula (ppm) Duplicates Remove'!$AH20</f>
         <v>6.7035728083648258E-2</v>
       </c>
-      <c r="AC19">
+      <c r="AB19">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC20*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG20))/'[1]Formula (ppm) Duplicates Remove'!$AH20</f>
         <v>0.42009056265752914</v>
       </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
       <c r="AD19">
-        <v>0</v>
-      </c>
-      <c r="AE19">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE20*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG20))/'[1]Formula (ppm) Duplicates Remove'!$AH20</f>
         <v>5.7337892754213806</v>
       </c>
-      <c r="AF19">
+      <c r="AE19">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF20*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG20))/'[1]Formula (ppm) Duplicates Remove'!$AH20</f>
         <v>0.22792147548440408</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -5616,73 +5555,70 @@
         <v>5.3600802094123381</v>
       </c>
       <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q21*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG21))/'[1]Formula (ppm) Duplicates Remove'!$AH21</f>
         <v>242.48266291828034</v>
       </c>
-      <c r="R20">
+      <c r="Q20">
         <f>'[1]Formula (ppm) Duplicates Remove'!R21*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG21))/'[1]Formula (ppm) Duplicates Remove'!$AH21</f>
         <v>3.3320090066866848</v>
       </c>
-      <c r="S20">
+      <c r="R20">
         <f>'[1]Formula (ppm) Duplicates Remove'!S21*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG21))/'[1]Formula (ppm) Duplicates Remove'!$AH21</f>
         <v>29.450579980684783</v>
       </c>
-      <c r="T20">
+      <c r="S20">
         <f>'[1]Formula (ppm) Duplicates Remove'!T21*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG21))/'[1]Formula (ppm) Duplicates Remove'!$AH21</f>
         <v>0.63206145459179841</v>
       </c>
-      <c r="U20">
+      <c r="T20">
         <f>'[1]Formula (ppm) Duplicates Remove'!U21*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG21))/'[1]Formula (ppm) Duplicates Remove'!$AH21</f>
         <v>2.5531301276030911</v>
       </c>
-      <c r="V20">
+      <c r="U20">
         <f>'[1]Formula (ppm) Duplicates Remove'!V21*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG21))/'[1]Formula (ppm) Duplicates Remove'!$AH21</f>
         <v>0.46284815178769484</v>
       </c>
-      <c r="W20">
+      <c r="V20">
         <f>'[1]Formula (ppm) Duplicates Remove'!W21*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG21))/'[1]Formula (ppm) Duplicates Remove'!$AH21</f>
         <v>0.15179428633897521</v>
       </c>
-      <c r="X20">
+      <c r="W20">
         <f>'[1]Formula (ppm) Duplicates Remove'!X21*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG21))/'[1]Formula (ppm) Duplicates Remove'!$AH21</f>
         <v>0.65694576382769609</v>
       </c>
-      <c r="Y20">
+      <c r="X20">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y21*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG21))/'[1]Formula (ppm) Duplicates Remove'!$AH21</f>
         <v>0.35086876022615576</v>
       </c>
-      <c r="Z20">
+      <c r="Y20">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z21*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG21))/'[1]Formula (ppm) Duplicates Remove'!$AH21</f>
         <v>8.4606651402051758E-2</v>
       </c>
-      <c r="AA20">
+      <c r="Z20">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA21*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG21))/'[1]Formula (ppm) Duplicates Remove'!$AH21</f>
         <v>0.20156290481077035</v>
       </c>
-      <c r="AB20">
+      <c r="AA20">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB21*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG21))/'[1]Formula (ppm) Duplicates Remove'!$AH21</f>
         <v>2.7372740159487333E-2</v>
       </c>
-      <c r="AC20">
+      <c r="AB20">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC21*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG21))/'[1]Formula (ppm) Duplicates Remove'!$AH21</f>
         <v>0.16672487188051377</v>
       </c>
+      <c r="AC20">
+        <v>0</v>
+      </c>
       <c r="AD20">
-        <v>0</v>
-      </c>
-      <c r="AE20">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE21*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG21))/'[1]Formula (ppm) Duplicates Remove'!$AH21</f>
         <v>4.8001832516046425</v>
       </c>
-      <c r="AF20">
+      <c r="AE20">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF21*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG21))/'[1]Formula (ppm) Duplicates Remove'!$AH21</f>
         <v>0.21898192127589866</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -5743,73 +5679,70 @@
         <v>10.768541861573711</v>
       </c>
       <c r="P21">
-        <v>0</v>
-      </c>
-      <c r="Q21">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q22*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG22))/'[1]Formula (ppm) Duplicates Remove'!$AH22</f>
         <v>16.849600795168278</v>
       </c>
-      <c r="R21">
+      <c r="Q21">
         <f>'[1]Formula (ppm) Duplicates Remove'!R22*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG22))/'[1]Formula (ppm) Duplicates Remove'!$AH22</f>
         <v>7.0349505310211651</v>
       </c>
-      <c r="S21">
+      <c r="R21">
         <f>'[1]Formula (ppm) Duplicates Remove'!S22*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG22))/'[1]Formula (ppm) Duplicates Remove'!$AH22</f>
         <v>77.447800205124437</v>
       </c>
-      <c r="T21">
+      <c r="S21">
         <f>'[1]Formula (ppm) Duplicates Remove'!T22*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG22))/'[1]Formula (ppm) Duplicates Remove'!$AH22</f>
         <v>1.5873352363426994</v>
       </c>
-      <c r="U21">
+      <c r="T21">
         <f>'[1]Formula (ppm) Duplicates Remove'!U22*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG22))/'[1]Formula (ppm) Duplicates Remove'!$AH22</f>
         <v>6.5170172027309423</v>
       </c>
-      <c r="V21">
+      <c r="U21">
         <f>'[1]Formula (ppm) Duplicates Remove'!V22*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG22))/'[1]Formula (ppm) Duplicates Remove'!$AH22</f>
         <v>1.2966963902517827</v>
       </c>
-      <c r="W21">
+      <c r="V21">
         <f>'[1]Formula (ppm) Duplicates Remove'!W22*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG22))/'[1]Formula (ppm) Duplicates Remove'!$AH22</f>
         <v>0.26455587272378317</v>
       </c>
-      <c r="X21">
+      <c r="W21">
         <f>'[1]Formula (ppm) Duplicates Remove'!X22*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG22))/'[1]Formula (ppm) Duplicates Remove'!$AH22</f>
         <v>1.7475592155979482</v>
       </c>
-      <c r="Y21">
+      <c r="X21">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y22*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG22))/'[1]Formula (ppm) Duplicates Remove'!$AH22</f>
         <v>1.0321405175279994</v>
       </c>
-      <c r="Z21">
+      <c r="Y21">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z22*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG22))/'[1]Formula (ppm) Duplicates Remove'!$AH22</f>
         <v>0.23102062125175438</v>
       </c>
-      <c r="AA21">
+      <c r="Z21">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA22*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG22))/'[1]Formula (ppm) Duplicates Remove'!$AH22</f>
         <v>0.56637313597204297</v>
       </c>
-      <c r="AB21">
+      <c r="AA21">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB22*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG22))/'[1]Formula (ppm) Duplicates Remove'!$AH22</f>
         <v>7.4522781048953032E-2</v>
       </c>
-      <c r="AC21">
+      <c r="AB21">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC22*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG22))/'[1]Formula (ppm) Duplicates Remove'!$AH22</f>
         <v>0.46949352060840405</v>
       </c>
+      <c r="AC21">
+        <v>0</v>
+      </c>
       <c r="AD21">
-        <v>0</v>
-      </c>
-      <c r="AE21">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE22*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG22))/'[1]Formula (ppm) Duplicates Remove'!$AH22</f>
         <v>2.9585544076434349</v>
       </c>
-      <c r="AF21">
+      <c r="AE21">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF22*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG22))/'[1]Formula (ppm) Duplicates Remove'!$AH22</f>
         <v>0.22729448219930673</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -5870,73 +5803,70 @@
         <v>38.051968132352975</v>
       </c>
       <c r="P22">
-        <v>0</v>
-      </c>
-      <c r="Q22">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q23*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG23))/'[1]Formula (ppm) Duplicates Remove'!$AH23</f>
         <v>421.87720473399349</v>
       </c>
-      <c r="R22">
+      <c r="Q22">
         <f>'[1]Formula (ppm) Duplicates Remove'!R23*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG23))/'[1]Formula (ppm) Duplicates Remove'!$AH23</f>
         <v>33.725803620908522</v>
       </c>
-      <c r="S22">
+      <c r="R22">
         <f>'[1]Formula (ppm) Duplicates Remove'!S23*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG23))/'[1]Formula (ppm) Duplicates Remove'!$AH23</f>
         <v>230.39872618168081</v>
       </c>
-      <c r="T22">
+      <c r="S22">
         <f>'[1]Formula (ppm) Duplicates Remove'!T23*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG23))/'[1]Formula (ppm) Duplicates Remove'!$AH23</f>
         <v>8.3629025238838199</v>
       </c>
-      <c r="U22">
+      <c r="T22">
         <f>'[1]Formula (ppm) Duplicates Remove'!U23*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG23))/'[1]Formula (ppm) Duplicates Remove'!$AH23</f>
         <v>36.208778322899526</v>
       </c>
-      <c r="V22">
+      <c r="U22">
         <f>'[1]Formula (ppm) Duplicates Remove'!V23*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG23))/'[1]Formula (ppm) Duplicates Remove'!$AH23</f>
         <v>8.0125441303513476</v>
       </c>
-      <c r="W22">
+      <c r="V22">
         <f>'[1]Formula (ppm) Duplicates Remove'!W23*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG23))/'[1]Formula (ppm) Duplicates Remove'!$AH23</f>
         <v>1.7974908885579066</v>
       </c>
-      <c r="X22">
+      <c r="W22">
         <f>'[1]Formula (ppm) Duplicates Remove'!X23*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG23))/'[1]Formula (ppm) Duplicates Remove'!$AH23</f>
         <v>9.566307440799708</v>
       </c>
-      <c r="Y22">
+      <c r="X22">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y23*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG23))/'[1]Formula (ppm) Duplicates Remove'!$AH23</f>
         <v>6.9919348970176207</v>
       </c>
-      <c r="Z22">
+      <c r="Y22">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z23*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG23))/'[1]Formula (ppm) Duplicates Remove'!$AH23</f>
         <v>1.6603941258712867</v>
       </c>
-      <c r="AA22">
+      <c r="Z22">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA23*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG23))/'[1]Formula (ppm) Duplicates Remove'!$AH23</f>
         <v>3.7473115134342807</v>
       </c>
-      <c r="AB22">
+      <c r="AA22">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB23*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG23))/'[1]Formula (ppm) Duplicates Remove'!$AH23</f>
         <v>0.50268812985094002</v>
       </c>
-      <c r="AC22">
+      <c r="AB22">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC23*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG23))/'[1]Formula (ppm) Duplicates Remove'!$AH23</f>
         <v>2.9704298582101001</v>
       </c>
+      <c r="AC22">
+        <v>0</v>
+      </c>
       <c r="AD22">
-        <v>0</v>
-      </c>
-      <c r="AE22">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE23*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG23))/'[1]Formula (ppm) Duplicates Remove'!$AH23</f>
         <v>30.801072683593961</v>
       </c>
-      <c r="AF22">
+      <c r="AE22">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF23*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG23))/'[1]Formula (ppm) Duplicates Remove'!$AH23</f>
         <v>1.5385303368165133</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -5997,73 +5927,70 @@
         <v>13.153065848594231</v>
       </c>
       <c r="P23">
-        <v>0</v>
-      </c>
-      <c r="Q23">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q24*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG24))/'[1]Formula (ppm) Duplicates Remove'!$AH24</f>
         <v>1426.4725119199159</v>
       </c>
-      <c r="R23">
+      <c r="Q23">
         <f>'[1]Formula (ppm) Duplicates Remove'!R24*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG24))/'[1]Formula (ppm) Duplicates Remove'!$AH24</f>
         <v>23.35567483311365</v>
       </c>
-      <c r="S23">
+      <c r="R23">
         <f>'[1]Formula (ppm) Duplicates Remove'!S24*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG24))/'[1]Formula (ppm) Duplicates Remove'!$AH24</f>
         <v>219.53322179537096</v>
       </c>
-      <c r="T23">
+      <c r="S23">
         <f>'[1]Formula (ppm) Duplicates Remove'!T24*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG24))/'[1]Formula (ppm) Duplicates Remove'!$AH24</f>
         <v>3.9828637256035631</v>
       </c>
-      <c r="U23">
+      <c r="T23">
         <f>'[1]Formula (ppm) Duplicates Remove'!U24*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG24))/'[1]Formula (ppm) Duplicates Remove'!$AH24</f>
         <v>14.853500679347468</v>
       </c>
-      <c r="V23">
+      <c r="U23">
         <f>'[1]Formula (ppm) Duplicates Remove'!V24*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG24))/'[1]Formula (ppm) Duplicates Remove'!$AH24</f>
         <v>2.6164428794625691</v>
       </c>
-      <c r="W23">
+      <c r="V23">
         <f>'[1]Formula (ppm) Duplicates Remove'!W24*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG24))/'[1]Formula (ppm) Duplicates Remove'!$AH24</f>
         <v>0.89070395896598098</v>
       </c>
-      <c r="X23">
+      <c r="W23">
         <f>'[1]Formula (ppm) Duplicates Remove'!X24*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG24))/'[1]Formula (ppm) Duplicates Remove'!$AH24</f>
         <v>4.124566628166332</v>
       </c>
-      <c r="Y23">
+      <c r="X23">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y24*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG24))/'[1]Formula (ppm) Duplicates Remove'!$AH24</f>
         <v>2.5101657025404918</v>
       </c>
-      <c r="Z23">
+      <c r="Y23">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z24*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG24))/'[1]Formula (ppm) Duplicates Remove'!$AH24</f>
         <v>0.55668997435373813</v>
       </c>
-      <c r="AA23">
+      <c r="Z23">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA24*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG24))/'[1]Formula (ppm) Duplicates Remove'!$AH24</f>
         <v>1.578975199985148</v>
       </c>
-      <c r="AB23">
+      <c r="AA23">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB24*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG24))/'[1]Formula (ppm) Duplicates Remove'!$AH24</f>
         <v>0.24291926153617663</v>
       </c>
-      <c r="AC23">
+      <c r="AB23">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC24*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG24))/'[1]Formula (ppm) Duplicates Remove'!$AH24</f>
         <v>1.6245225615231813</v>
       </c>
+      <c r="AC23">
+        <v>0</v>
+      </c>
       <c r="AD23">
-        <v>0</v>
-      </c>
-      <c r="AE23">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE24*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG24))/'[1]Formula (ppm) Duplicates Remove'!$AH24</f>
         <v>22.308085517738892</v>
       </c>
-      <c r="AF23">
+      <c r="AE23">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF24*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG24))/'[1]Formula (ppm) Duplicates Remove'!$AH24</f>
         <v>0.59211569999443059</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -6124,73 +6051,70 @@
         <v>11.164679670982512</v>
       </c>
       <c r="P24">
-        <v>0</v>
-      </c>
-      <c r="Q24">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q25*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG25))/'[1]Formula (ppm) Duplicates Remove'!$AH25</f>
         <v>774.08251076558406</v>
       </c>
-      <c r="R24">
+      <c r="Q24">
         <f>'[1]Formula (ppm) Duplicates Remove'!R25*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG25))/'[1]Formula (ppm) Duplicates Remove'!$AH25</f>
         <v>24.571638104338081</v>
       </c>
-      <c r="S24">
+      <c r="R24">
         <f>'[1]Formula (ppm) Duplicates Remove'!S25*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG25))/'[1]Formula (ppm) Duplicates Remove'!$AH25</f>
         <v>153.572738152113</v>
       </c>
-      <c r="T24">
+      <c r="S24">
         <f>'[1]Formula (ppm) Duplicates Remove'!T25*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG25))/'[1]Formula (ppm) Duplicates Remove'!$AH25</f>
         <v>3.795523946725226</v>
       </c>
-      <c r="U24">
+      <c r="T24">
         <f>'[1]Formula (ppm) Duplicates Remove'!U25*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG25))/'[1]Formula (ppm) Duplicates Remove'!$AH25</f>
         <v>14.189420293142003</v>
       </c>
-      <c r="V24">
+      <c r="U24">
         <f>'[1]Formula (ppm) Duplicates Remove'!V25*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG25))/'[1]Formula (ppm) Duplicates Remove'!$AH25</f>
         <v>2.5634384809421142</v>
       </c>
-      <c r="W24">
+      <c r="V24">
         <f>'[1]Formula (ppm) Duplicates Remove'!W25*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG25))/'[1]Formula (ppm) Duplicates Remove'!$AH25</f>
         <v>0.70071211324158023</v>
       </c>
-      <c r="X24">
+      <c r="W24">
         <f>'[1]Formula (ppm) Duplicates Remove'!X25*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG25))/'[1]Formula (ppm) Duplicates Remove'!$AH25</f>
         <v>3.6437029888562171</v>
       </c>
-      <c r="Y24">
+      <c r="X24">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y25*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG25))/'[1]Formula (ppm) Duplicates Remove'!$AH25</f>
         <v>2.2597965652040966</v>
       </c>
-      <c r="Z24">
+      <c r="Y24">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z25*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG25))/'[1]Formula (ppm) Duplicates Remove'!$AH25</f>
         <v>0.57808749342430377</v>
       </c>
-      <c r="AA24">
+      <c r="Z24">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA25*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG25))/'[1]Formula (ppm) Duplicates Remove'!$AH25</f>
         <v>1.3605493532107351</v>
       </c>
-      <c r="AB24">
+      <c r="AA24">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB25*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG25))/'[1]Formula (ppm) Duplicates Remove'!$AH25</f>
         <v>0.18685656353108807</v>
       </c>
-      <c r="AC24">
+      <c r="AB24">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC25*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG25))/'[1]Formula (ppm) Duplicates Remove'!$AH25</f>
         <v>1.3371922827693492</v>
       </c>
+      <c r="AC24">
+        <v>0</v>
+      </c>
       <c r="AD24">
-        <v>0</v>
-      </c>
-      <c r="AE24">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE25*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG25))/'[1]Formula (ppm) Duplicates Remove'!$AH25</f>
         <v>41.452960765849824</v>
       </c>
-      <c r="AF24">
+      <c r="AE24">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF25*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG25))/'[1]Formula (ppm) Duplicates Remove'!$AH25</f>
         <v>1.8568871000901881</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -6251,73 +6175,70 @@
         <v>13.802596491085877</v>
       </c>
       <c r="P25">
-        <v>0</v>
-      </c>
-      <c r="Q25">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q26*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG26))/'[1]Formula (ppm) Duplicates Remove'!$AH26</f>
         <v>49.50553028303969</v>
       </c>
-      <c r="R25">
+      <c r="Q25">
         <f>'[1]Formula (ppm) Duplicates Remove'!R26*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG26))/'[1]Formula (ppm) Duplicates Remove'!$AH26</f>
         <v>3.6872184479732959</v>
       </c>
-      <c r="S25">
+      <c r="R25">
         <f>'[1]Formula (ppm) Duplicates Remove'!S26*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG26))/'[1]Formula (ppm) Duplicates Remove'!$AH26</f>
         <v>19.627096428813601</v>
       </c>
-      <c r="T25">
+      <c r="S25">
         <f>'[1]Formula (ppm) Duplicates Remove'!T26*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG26))/'[1]Formula (ppm) Duplicates Remove'!$AH26</f>
         <v>0.85926329613536978</v>
       </c>
-      <c r="U25">
+      <c r="T25">
         <f>'[1]Formula (ppm) Duplicates Remove'!U26*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG26))/'[1]Formula (ppm) Duplicates Remove'!$AH26</f>
         <v>3.5186288139214188</v>
       </c>
-      <c r="V25">
+      <c r="U25">
         <f>'[1]Formula (ppm) Duplicates Remove'!V26*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG26))/'[1]Formula (ppm) Duplicates Remove'!$AH26</f>
         <v>0.74505741500345357</v>
       </c>
-      <c r="W25">
+      <c r="V25">
         <f>'[1]Formula (ppm) Duplicates Remove'!W26*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG26))/'[1]Formula (ppm) Duplicates Remove'!$AH26</f>
         <v>0.16315125875988032</v>
       </c>
-      <c r="X25">
+      <c r="W25">
         <f>'[1]Formula (ppm) Duplicates Remove'!X26*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG26))/'[1]Formula (ppm) Duplicates Remove'!$AH26</f>
         <v>0.7940027926314176</v>
       </c>
-      <c r="Y25">
+      <c r="X25">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y26*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG26))/'[1]Formula (ppm) Duplicates Remove'!$AH26</f>
         <v>0.7341806644194615</v>
       </c>
-      <c r="Z25">
+      <c r="Y25">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z26*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG26))/'[1]Formula (ppm) Duplicates Remove'!$AH26</f>
         <v>0.1903431352198604</v>
       </c>
-      <c r="AA25">
+      <c r="Z25">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA26*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG26))/'[1]Formula (ppm) Duplicates Remove'!$AH26</f>
         <v>0.47313865040365294</v>
       </c>
-      <c r="AB25">
+      <c r="AA25">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB26*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG26))/'[1]Formula (ppm) Duplicates Remove'!$AH26</f>
         <v>6.5260503503952141E-2</v>
       </c>
-      <c r="AC25">
+      <c r="AB25">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC26*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG26))/'[1]Formula (ppm) Duplicates Remove'!$AH26</f>
         <v>0.41331652219169684</v>
       </c>
+      <c r="AC25">
+        <v>0</v>
+      </c>
       <c r="AD25">
-        <v>0</v>
-      </c>
-      <c r="AE25">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE26*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG26))/'[1]Formula (ppm) Duplicates Remove'!$AH26</f>
         <v>9.3322520010651555</v>
       </c>
-      <c r="AF25">
+      <c r="AE25">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF26*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG26))/'[1]Formula (ppm) Duplicates Remove'!$AH26</f>
         <v>1.8109789722346719</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -6378,73 +6299,70 @@
         <v>6.0400476764164202</v>
       </c>
       <c r="P26">
-        <v>0</v>
-      </c>
-      <c r="Q26">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q27*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG27))/'[1]Formula (ppm) Duplicates Remove'!$AH27</f>
         <v>480.6958592303248</v>
       </c>
-      <c r="R26">
+      <c r="Q26">
         <f>'[1]Formula (ppm) Duplicates Remove'!R27*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG27))/'[1]Formula (ppm) Duplicates Remove'!$AH27</f>
         <v>15.095049201385416</v>
       </c>
-      <c r="S26">
+      <c r="R26">
         <f>'[1]Formula (ppm) Duplicates Remove'!S27*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG27))/'[1]Formula (ppm) Duplicates Remove'!$AH27</f>
         <v>81.386853945400659</v>
       </c>
-      <c r="T26">
+      <c r="S26">
         <f>'[1]Formula (ppm) Duplicates Remove'!T27*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG27))/'[1]Formula (ppm) Duplicates Remove'!$AH27</f>
         <v>3.1366336002878787</v>
       </c>
-      <c r="U26">
+      <c r="T26">
         <f>'[1]Formula (ppm) Duplicates Remove'!U27*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG27))/'[1]Formula (ppm) Duplicates Remove'!$AH27</f>
         <v>13.607852235731679</v>
       </c>
-      <c r="V26">
+      <c r="U26">
         <f>'[1]Formula (ppm) Duplicates Remove'!V27*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG27))/'[1]Formula (ppm) Duplicates Remove'!$AH27</f>
         <v>2.9743939313074708</v>
       </c>
-      <c r="W26">
+      <c r="V26">
         <f>'[1]Formula (ppm) Duplicates Remove'!W27*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG27))/'[1]Formula (ppm) Duplicates Remove'!$AH27</f>
         <v>0.77063842765693569</v>
       </c>
-      <c r="X26">
+      <c r="W26">
         <f>'[1]Formula (ppm) Duplicates Remove'!X27*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG27))/'[1]Formula (ppm) Duplicates Remove'!$AH27</f>
         <v>3.71461242103058</v>
       </c>
-      <c r="Y26">
+      <c r="X26">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y27*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG27))/'[1]Formula (ppm) Duplicates Remove'!$AH27</f>
         <v>2.9169340485435762</v>
       </c>
-      <c r="Z26">
+      <c r="Y26">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z27*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG27))/'[1]Formula (ppm) Duplicates Remove'!$AH27</f>
         <v>0.66585864144042251</v>
       </c>
-      <c r="AA26">
+      <c r="Z26">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA27*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG27))/'[1]Formula (ppm) Duplicates Remove'!$AH27</f>
         <v>1.6528166277379013</v>
       </c>
-      <c r="AB26">
+      <c r="AA26">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB27*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG27))/'[1]Formula (ppm) Duplicates Remove'!$AH27</f>
         <v>0.21969955174430186</v>
       </c>
-      <c r="AC26">
+      <c r="AB26">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC27*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG27))/'[1]Formula (ppm) Duplicates Remove'!$AH27</f>
         <v>1.4026971380597733</v>
       </c>
+      <c r="AC26">
+        <v>0</v>
+      </c>
       <c r="AD26">
-        <v>0</v>
-      </c>
-      <c r="AE26">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE27*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG27))/'[1]Formula (ppm) Duplicates Remove'!$AH27</f>
         <v>28.199282464657077</v>
       </c>
-      <c r="AF26">
+      <c r="AE26">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF27*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG27))/'[1]Formula (ppm) Duplicates Remove'!$AH27</f>
         <v>1.375657193229705</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -6505,68 +6423,65 @@
         <v>1.0129996365724523</v>
       </c>
       <c r="P27">
-        <v>0</v>
-      </c>
-      <c r="Q27">
         <f>'[1]Formula (ppm) Duplicates Remove'!Q28*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG28))/'[1]Formula (ppm) Duplicates Remove'!$AH28</f>
         <v>95.646278893129548</v>
       </c>
-      <c r="R27">
+      <c r="Q27">
         <f>'[1]Formula (ppm) Duplicates Remove'!R28*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG28))/'[1]Formula (ppm) Duplicates Remove'!$AH28</f>
         <v>8.3562913416882303</v>
       </c>
-      <c r="S27">
+      <c r="R27">
         <f>'[1]Formula (ppm) Duplicates Remove'!S28*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG28))/'[1]Formula (ppm) Duplicates Remove'!$AH28</f>
         <v>38.673650276239627</v>
       </c>
-      <c r="T27">
+      <c r="S27">
         <f>'[1]Formula (ppm) Duplicates Remove'!T28*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG28))/'[1]Formula (ppm) Duplicates Remove'!$AH28</f>
         <v>1.5825730171358312</v>
       </c>
-      <c r="U27">
+      <c r="T27">
         <f>'[1]Formula (ppm) Duplicates Remove'!U28*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG28))/'[1]Formula (ppm) Duplicates Remove'!$AH28</f>
         <v>6.0894657398487428</v>
       </c>
-      <c r="V27">
+      <c r="U27">
         <f>'[1]Formula (ppm) Duplicates Remove'!V28*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG28))/'[1]Formula (ppm) Duplicates Remove'!$AH28</f>
         <v>1.1276788407127298</v>
       </c>
-      <c r="W27">
+      <c r="V27">
         <f>'[1]Formula (ppm) Duplicates Remove'!W28*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG28))/'[1]Formula (ppm) Duplicates Remove'!$AH28</f>
         <v>0.26376216952263859</v>
       </c>
-      <c r="X27">
+      <c r="W27">
         <f>'[1]Formula (ppm) Duplicates Remove'!X28*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG28))/'[1]Formula (ppm) Duplicates Remove'!$AH28</f>
         <v>1.425844771477452</v>
       </c>
-      <c r="Y27">
+      <c r="X27">
         <f>'[1]Formula (ppm) Duplicates Remove'!Y28*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG28))/'[1]Formula (ppm) Duplicates Remove'!$AH28</f>
         <v>1.1506146815407856</v>
       </c>
-      <c r="Z27">
+      <c r="Y27">
         <f>'[1]Formula (ppm) Duplicates Remove'!Z28*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG28))/'[1]Formula (ppm) Duplicates Remove'!$AH28</f>
         <v>0.27523008993666626</v>
       </c>
-      <c r="AA27">
+      <c r="Z27">
         <f>'[1]Formula (ppm) Duplicates Remove'!AA28*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG28))/'[1]Formula (ppm) Duplicates Remove'!$AH28</f>
         <v>0.79510914870592475</v>
       </c>
-      <c r="AB27">
+      <c r="AA27">
         <f>'[1]Formula (ppm) Duplicates Remove'!AB28*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG28))/'[1]Formula (ppm) Duplicates Remove'!$AH28</f>
         <v>0.11085656400226838</v>
       </c>
-      <c r="AC27">
+      <c r="AB27">
         <f>'[1]Formula (ppm) Duplicates Remove'!AC28*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG28))/'[1]Formula (ppm) Duplicates Remove'!$AH28</f>
         <v>0.71483370580773054</v>
       </c>
+      <c r="AC27">
+        <v>0</v>
+      </c>
       <c r="AD27">
-        <v>0</v>
-      </c>
-      <c r="AE27">
         <f>'[1]Formula (ppm) Duplicates Remove'!AE28*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG28))/'[1]Formula (ppm) Duplicates Remove'!$AH28</f>
         <v>5.9403827744663804</v>
       </c>
-      <c r="AF27">
+      <c r="AE27">
         <f>'[1]Formula (ppm) Duplicates Remove'!AF28*(400435-(85475*'[1]Formula (ppm) Duplicates Remove'!$AG28))/'[1]Formula (ppm) Duplicates Remove'!$AH28</f>
         <v>0.73012426635976757</v>
       </c>
@@ -6580,7 +6495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F2BC39-F234-4290-807E-B62380110B4E}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -6594,7 +6509,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -6602,7 +6517,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -6610,7 +6525,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -6618,15 +6533,15 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -6634,7 +6549,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -6642,15 +6557,15 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" t="s">
         <v>77</v>
-      </c>
-      <c r="B8" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -6658,7 +6573,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -6666,7 +6581,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -6674,7 +6589,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -6682,39 +6597,39 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -6722,7 +6637,7 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -6730,23 +6645,23 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -6754,23 +6669,23 @@
         <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" t="s">
         <v>80</v>
-      </c>
-      <c r="B23" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -6778,7 +6693,7 @@
         <v>13</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -6786,7 +6701,7 @@
         <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -6794,23 +6709,23 @@
         <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -6818,7 +6733,7 @@
         <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -6826,7 +6741,7 @@
         <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -6834,7 +6749,7 @@
         <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -6842,7 +6757,7 @@
         <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -6850,7 +6765,7 @@
         <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -6858,7 +6773,7 @@
         <v>21</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -6866,23 +6781,23 @@
         <v>22</v>
       </c>
       <c r="B35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -6890,7 +6805,7 @@
         <v>23</v>
       </c>
       <c r="B38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -6898,7 +6813,7 @@
         <v>24</v>
       </c>
       <c r="B39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -6906,7 +6821,7 @@
         <v>25</v>
       </c>
       <c r="B40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -6914,7 +6829,7 @@
         <v>26</v>
       </c>
       <c r="B41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>